<commit_message>
plots are broken, aaaaaaaaaaaaaaaaaa
</commit_message>
<xml_diff>
--- a/output/LUAD_statistics_.xlsx
+++ b/output/LUAD_statistics_.xlsx
@@ -57,48 +57,51 @@
     <t>5</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
     <t>17</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>27</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>10</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -108,9 +111,6 @@
     <t>31</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -216,36 +216,36 @@
     <t>Mutation EGFR</t>
   </si>
   <si>
+    <t>Pattern OR_CDK4_TP53</t>
+  </si>
+  <si>
+    <t>Mutation TP53</t>
+  </si>
+  <si>
+    <t>Mutation KRAS</t>
+  </si>
+  <si>
+    <t>Amplification CDK4</t>
+  </si>
+  <si>
     <t>Pattern OR_KRAS</t>
   </si>
   <si>
-    <t>Mutation TP53</t>
-  </si>
-  <si>
-    <t>Pattern OR_CDK4_TP53</t>
-  </si>
-  <si>
     <t>Mutation ATM</t>
   </si>
   <si>
+    <t>Mutation SMARCA4</t>
+  </si>
+  <si>
     <t>Pattern OR_CDKN2A</t>
   </si>
   <si>
-    <t>Amplification CDK4</t>
-  </si>
-  <si>
-    <t>Mutation SMARCA4</t>
+    <t>Mutation KEAP1</t>
   </si>
   <si>
     <t>Mutation ARID2</t>
   </si>
   <si>
-    <t>Mutation KRAS</t>
-  </si>
-  <si>
-    <t>Mutation KEAP1</t>
-  </si>
-  <si>
     <t>Pattern OR_EGFR_SMARCA4</t>
   </si>
   <si>
@@ -261,24 +261,27 @@
     <t>Mutation RB1</t>
   </si>
   <si>
+    <t>Amplification KRAS</t>
+  </si>
+  <si>
+    <t>Amplification MDM2</t>
+  </si>
+  <si>
+    <t>Amplification CCND1</t>
+  </si>
+  <si>
+    <t>Mutation NFE2L2</t>
+  </si>
+  <si>
     <t>Mutation STK11</t>
   </si>
   <si>
-    <t>Amplification CCND1</t>
-  </si>
-  <si>
-    <t>Amplification KRAS</t>
+    <t>Amplification MET</t>
   </si>
   <si>
     <t>Mutation CDKN2A</t>
   </si>
   <si>
-    <t>Amplification MDM2</t>
-  </si>
-  <si>
-    <t>Mutation NFE2L2</t>
-  </si>
-  <si>
     <t>Pattern AND_PIK3CA_RB1</t>
   </si>
   <si>
@@ -291,9 +294,6 @@
     <t>Mutation RET</t>
   </si>
   <si>
-    <t>Amplification MET</t>
-  </si>
-  <si>
     <t>Amplification CCNE1</t>
   </si>
   <si>
@@ -405,10 +405,10 @@
     <t>58</t>
   </si>
   <si>
+    <t>57</t>
+  </si>
+  <si>
     <t>60</t>
-  </si>
-  <si>
-    <t>57</t>
   </si>
   <si>
     <t>54</t>
@@ -610,22 +610,22 @@
         <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D3" t="n">
-        <v>158.0</v>
+        <v>265.0</v>
       </c>
       <c r="E3" t="n">
-        <v>46.0</v>
+        <v>28.0</v>
       </c>
       <c r="F3" t="n">
-        <v>3.96357880596532E-5</v>
+        <v>3.94511214512808E-5</v>
       </c>
       <c r="G3" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00152282025112865</v>
+        <v>4.62083488900288E-6</v>
       </c>
       <c r="I3" t="n">
         <v>90.0</v>
@@ -634,13 +634,13 @@
         <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L3" t="n">
         <v>0.0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N3" t="n">
         <v>0.0</v>
@@ -672,7 +672,7 @@
         <v>7.08630770929278E-6</v>
       </c>
       <c r="I4" t="n">
-        <v>90.0</v>
+        <v>80.0</v>
       </c>
       <c r="J4" t="n">
         <v>100.0</v>
@@ -681,13 +681,13 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L4" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M4" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N4" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -698,40 +698,40 @@
         <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D5" t="n">
-        <v>265.0</v>
+        <v>141.0</v>
       </c>
       <c r="E5" t="n">
-        <v>28.0</v>
+        <v>34.0</v>
       </c>
       <c r="F5" t="n">
-        <v>3.94511214512808E-5</v>
+        <v>4.01937482104294E-5</v>
       </c>
       <c r="G5" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H5" t="n">
-        <v>4.62083488900288E-6</v>
+        <v>0.00103577594631515</v>
       </c>
       <c r="I5" t="n">
-        <v>80.0</v>
+        <v>70.0</v>
       </c>
       <c r="J5" t="n">
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L5" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N5" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -739,43 +739,43 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D6" t="n">
-        <v>158.0</v>
+        <v>29.0</v>
       </c>
       <c r="E6" t="n">
-        <v>84.0</v>
+        <v>26.0</v>
       </c>
       <c r="F6" t="n">
-        <v>3.96357880596532E-5</v>
+        <v>0.00799712708568516</v>
       </c>
       <c r="G6" t="n">
-        <v>1.4175710770138E-6</v>
+        <v>4.03810600803007E-5</v>
       </c>
       <c r="H6" t="n">
-        <v>8.72881864945047E-5</v>
+        <v>1.22060965342091E-9</v>
       </c>
       <c r="I6" t="n">
-        <v>80.0</v>
+        <v>70.0</v>
       </c>
       <c r="J6" t="n">
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1784355179704017</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0026742305794235717</v>
+        <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="7">
@@ -783,40 +783,40 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D7" t="n">
+        <v>158.0</v>
+      </c>
+      <c r="E7" t="n">
         <v>46.0</v>
       </c>
-      <c r="E7" t="n">
-        <v>19.0</v>
-      </c>
       <c r="F7" t="n">
-        <v>3.98211137138711E-5</v>
+        <v>3.96357880596532E-5</v>
       </c>
       <c r="G7" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00625718664081437</v>
+        <v>0.00152282025112865</v>
       </c>
       <c r="I7" t="n">
-        <v>70.0</v>
+        <v>60.0</v>
       </c>
       <c r="J7" t="n">
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.040169133192389</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L7" t="n">
         <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -827,40 +827,40 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>84</v>
       </c>
       <c r="D8" t="n">
-        <v>265.0</v>
+        <v>46.0</v>
       </c>
       <c r="E8" t="n">
-        <v>34.0</v>
+        <v>19.0</v>
       </c>
       <c r="F8" t="n">
-        <v>4.03810600803007E-5</v>
+        <v>3.98211137138711E-5</v>
       </c>
       <c r="G8" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H8" t="n">
-        <v>5.41340370300314E-5</v>
+        <v>0.00625718664081437</v>
       </c>
       <c r="I8" t="n">
-        <v>70.0</v>
+        <v>50.0</v>
       </c>
       <c r="J8" t="n">
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N8" t="n">
         <v>0.0</v>
@@ -871,40 +871,40 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D9" t="n">
-        <v>250.0</v>
+        <v>265.0</v>
       </c>
       <c r="E9" t="n">
-        <v>25.0</v>
+        <v>34.0</v>
       </c>
       <c r="F9" t="n">
-        <v>3.98211137138711E-5</v>
+        <v>4.03810600803007E-5</v>
       </c>
       <c r="G9" t="n">
-        <v>9.92299753909661E-6</v>
+        <v>1.4175710770138E-6</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00470560456401602</v>
+        <v>5.41340370300314E-5</v>
       </c>
       <c r="I9" t="n">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c r="J9" t="n">
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -915,25 +915,25 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D10" t="n">
-        <v>103.0</v>
+        <v>48.0</v>
       </c>
       <c r="E10" t="n">
-        <v>19.0</v>
+        <v>15.0</v>
       </c>
       <c r="F10" t="n">
-        <v>3.98211137138711E-5</v>
+        <v>3.83568771824305E-5</v>
       </c>
       <c r="G10" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H10" t="n">
-        <v>4.20631113667766E-4</v>
+        <v>0.00180163808571658</v>
       </c>
       <c r="I10" t="n">
         <v>50.0</v>
@@ -942,13 +942,13 @@
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.040169133192389</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -959,40 +959,40 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
         <v>86</v>
       </c>
       <c r="D11" t="n">
-        <v>29.0</v>
+        <v>158.0</v>
       </c>
       <c r="E11" t="n">
-        <v>26.0</v>
+        <v>84.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00799712708568516</v>
+        <v>3.96357880596532E-5</v>
       </c>
       <c r="G11" t="n">
-        <v>4.03810600803007E-5</v>
+        <v>1.4175710770138E-6</v>
       </c>
       <c r="H11" t="n">
-        <v>1.22060965342091E-9</v>
+        <v>8.72881864945047E-5</v>
       </c>
       <c r="I11" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="J11" t="n">
         <v>100.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.17864693446088797</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0</v>
+        <v>0.002283559090348079</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N11" t="n">
         <v>0.0</v>
@@ -1003,40 +1003,40 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D12" t="n">
-        <v>250.0</v>
+        <v>103.0</v>
       </c>
       <c r="E12" t="n">
-        <v>26.0</v>
+        <v>15.0</v>
       </c>
       <c r="F12" t="n">
-        <v>3.98211137138711E-5</v>
+        <v>3.96357880596532E-5</v>
       </c>
       <c r="G12" t="n">
-        <v>1.4175710770138E-6</v>
+        <v>9.05702480294115E-5</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00470560456401602</v>
+        <v>0.00920956456293582</v>
       </c>
       <c r="I12" t="n">
-        <v>50.0</v>
+        <v>30.0</v>
       </c>
       <c r="J12" t="n">
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N12" t="n">
         <v>0.0</v>
@@ -1047,40 +1047,40 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D13" t="n">
-        <v>48.0</v>
+        <v>250.0</v>
       </c>
       <c r="E13" t="n">
-        <v>15.0</v>
+        <v>25.0</v>
       </c>
       <c r="F13" t="n">
-        <v>3.83568771824305E-5</v>
+        <v>3.98211137138711E-5</v>
       </c>
       <c r="G13" t="n">
-        <v>1.4175710770138E-6</v>
+        <v>9.92299753909661E-6</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00180163808571658</v>
+        <v>0.00470560456401602</v>
       </c>
       <c r="I13" t="n">
-        <v>40.0</v>
+        <v>30.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N13" t="n">
         <v>0.0</v>
@@ -1091,40 +1091,40 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D14" t="n">
-        <v>32.0</v>
+        <v>250.0</v>
       </c>
       <c r="E14" t="n">
-        <v>2.0</v>
+        <v>26.0</v>
       </c>
       <c r="F14" t="n">
-        <v>3.64111620331533E-5</v>
+        <v>3.98211137138711E-5</v>
       </c>
       <c r="G14" t="n">
-        <v>3.14719354078108E-5</v>
+        <v>1.4175710770138E-6</v>
       </c>
       <c r="H14" t="n">
-        <v>0.00389687175260687</v>
+        <v>0.00470560456401602</v>
       </c>
       <c r="I14" t="n">
-        <v>40.0</v>
+        <v>30.0</v>
       </c>
       <c r="J14" t="n">
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.004228329809725159</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M14" t="n">
-        <v>0.00422832980972516</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N14" t="n">
         <v>0.0</v>
@@ -1138,22 +1138,22 @@
         <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D15" t="n">
-        <v>141.0</v>
+        <v>93.0</v>
       </c>
       <c r="E15" t="n">
-        <v>34.0</v>
+        <v>84.0</v>
       </c>
       <c r="F15" t="n">
-        <v>4.01937482104294E-5</v>
+        <v>0.00260366851725413</v>
       </c>
       <c r="G15" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H15" t="n">
-        <v>0.00103577594631515</v>
+        <v>2.66335709542836E-4</v>
       </c>
       <c r="I15" t="n">
         <v>30.0</v>
@@ -1162,13 +1162,13 @@
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.17864693446088797</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0</v>
+        <v>0.002283559090348079</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -1182,22 +1182,22 @@
         <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D16" t="n">
-        <v>93.0</v>
+        <v>32.0</v>
       </c>
       <c r="E16" t="n">
-        <v>84.0</v>
+        <v>2.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.00260366851725413</v>
+        <v>3.64111620331533E-5</v>
       </c>
       <c r="G16" t="n">
-        <v>1.4175710770138E-6</v>
+        <v>3.14719354078108E-5</v>
       </c>
       <c r="H16" t="n">
-        <v>2.66335709542836E-4</v>
+        <v>0.00389687175260687</v>
       </c>
       <c r="I16" t="n">
         <v>30.0</v>
@@ -1206,13 +1206,13 @@
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1784355179704017</v>
+        <v>0.004228329809725159</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0026742305794235717</v>
+        <v>0.0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.177589852008457</v>
+        <v>0.00422832980972516</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -1223,25 +1223,25 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D17" t="n">
-        <v>120.0</v>
+        <v>103.0</v>
       </c>
       <c r="E17" t="n">
-        <v>82.0</v>
+        <v>19.0</v>
       </c>
       <c r="F17" t="n">
-        <v>3.94511214512808E-5</v>
+        <v>3.98211137138711E-5</v>
       </c>
       <c r="G17" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H17" t="n">
-        <v>0.00112197360386636</v>
+        <v>4.20631113667766E-4</v>
       </c>
       <c r="I17" t="n">
         <v>20.0</v>
@@ -1250,13 +1250,13 @@
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.173361522198731</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -1267,25 +1267,25 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>
       </c>
       <c r="D18" t="n">
-        <v>26.0</v>
+        <v>120.0</v>
       </c>
       <c r="E18" t="n">
-        <v>25.0</v>
+        <v>82.0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.152526861987935</v>
+        <v>3.94511214512808E-5</v>
       </c>
       <c r="G18" t="n">
-        <v>5.32401707922167E-5</v>
+        <v>1.4175710770138E-6</v>
       </c>
       <c r="H18" t="n">
-        <v>4.94689940303263E-4</v>
+        <v>0.00112197360386636</v>
       </c>
       <c r="I18" t="n">
         <v>20.0</v>
@@ -1294,16 +1294,16 @@
         <v>100.0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L18" t="n">
         <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N18" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
@@ -1311,25 +1311,25 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
       </c>
       <c r="D19" t="n">
-        <v>265.0</v>
+        <v>26.0</v>
       </c>
       <c r="E19" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="F19" t="n">
-        <v>4.00070999263567E-5</v>
+        <v>0.152526861987935</v>
       </c>
       <c r="G19" t="n">
-        <v>4.05690370510693E-5</v>
+        <v>5.32401707922167E-5</v>
       </c>
       <c r="H19" t="n">
-        <v>2.49022843057501E-4</v>
+        <v>4.94689940303263E-4</v>
       </c>
       <c r="I19" t="n">
         <v>20.0</v>
@@ -1338,16 +1338,16 @@
         <v>100.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L19" t="n">
         <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N19" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -1355,40 +1355,40 @@
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>92</v>
       </c>
       <c r="D20" t="n">
-        <v>103.0</v>
+        <v>265.0</v>
       </c>
       <c r="E20" t="n">
-        <v>15.0</v>
+        <v>23.0</v>
       </c>
       <c r="F20" t="n">
-        <v>3.96357880596532E-5</v>
+        <v>4.00070999263567E-5</v>
       </c>
       <c r="G20" t="n">
-        <v>9.05702480294115E-5</v>
+        <v>4.05690370510693E-5</v>
       </c>
       <c r="H20" t="n">
-        <v>0.00920956456293582</v>
+        <v>2.49022843057501E-4</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="J20" t="n">
         <v>100.0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L20" t="n">
         <v>0.0</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N20" t="n">
         <v>0.0</v>
@@ -1429,7 +1429,7 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L21" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M21" t="e">
         <v>#NUM!</v>
@@ -1446,7 +1446,7 @@
         <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D22" t="e">
         <v>#NUM!</v>
@@ -1517,7 +1517,7 @@
         <v>0.12473572938689217</v>
       </c>
       <c r="L23" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M23" t="e">
         <v>#NUM!</v>
@@ -1605,7 +1605,7 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M25" t="e">
         <v>#NUM!</v>
@@ -1622,7 +1622,7 @@
         <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D26" t="e">
         <v>#NUM!</v>
@@ -1798,7 +1798,7 @@
         <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" t="e">
         <v>#NUM!</v>
@@ -1842,7 +1842,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D31" t="e">
         <v>#NUM!</v>
@@ -1957,7 +1957,7 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L33" t="n">
-        <v>8.012344526598183E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M33" t="e">
         <v>#NUM!</v>
@@ -2045,7 +2045,7 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L35" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M35" t="e">
         <v>#NUM!</v>
@@ -2326,7 +2326,7 @@
         <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D42" t="e">
         <v>#NUM!</v>
@@ -2370,7 +2370,7 @@
         <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D43" t="e">
         <v>#NUM!</v>
@@ -2482,10 +2482,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K45" t="n">
-        <v>0.48773784355179706</v>
+        <v>0.48520084566596194</v>
       </c>
       <c r="L45" t="n">
-        <v>0.0067631250818943524</v>
+        <v>0.003342788224279473</v>
       </c>
       <c r="M45" t="e">
         <v>#NUM!</v>
@@ -2634,7 +2634,7 @@
         <v>79</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D49" t="e">
         <v>#NUM!</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>66</v>
@@ -2983,36 +2983,36 @@
         <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.12262156448203</v>
+        <v>0.125581395348837</v>
       </c>
       <c r="N2" t="n">
-        <v>0.00645888047210125</v>
+        <v>0.00565536367800955</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D3" t="n">
-        <v>158.0</v>
+        <v>265.0</v>
       </c>
       <c r="E3" t="n">
-        <v>46.0</v>
+        <v>28.0</v>
       </c>
       <c r="F3" t="n">
-        <v>3.96357880596532E-5</v>
+        <v>3.94511214512808E-5</v>
       </c>
       <c r="G3" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H3" t="n">
-        <v>0.00152282025112865</v>
+        <v>4.62083488900288E-6</v>
       </c>
       <c r="I3" t="n">
         <v>90.0</v>
@@ -3021,13 +3021,13 @@
         <v>100.0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L3" t="n">
         <v>0.0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N3" t="n">
         <v>0.0</v>
@@ -3059,7 +3059,7 @@
         <v>7.08630770929278E-6</v>
       </c>
       <c r="I4" t="n">
-        <v>90.0</v>
+        <v>80.0</v>
       </c>
       <c r="J4" t="n">
         <v>100.0</v>
@@ -3068,98 +3068,98 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L4" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M4" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N4" t="n">
-        <v>6.5420519111824E-18</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D5" t="n">
-        <v>265.0</v>
+        <v>141.0</v>
       </c>
       <c r="E5" t="n">
-        <v>28.0</v>
+        <v>34.0</v>
       </c>
       <c r="F5" t="n">
-        <v>3.94511214512808E-5</v>
+        <v>4.01937482104294E-5</v>
       </c>
       <c r="G5" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H5" t="n">
-        <v>4.62083488900288E-6</v>
+        <v>0.00103577594631515</v>
       </c>
       <c r="I5" t="n">
-        <v>80.0</v>
+        <v>70.0</v>
       </c>
       <c r="J5" t="n">
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L5" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N5" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D6" t="n">
-        <v>158.0</v>
+        <v>29.0</v>
       </c>
       <c r="E6" t="n">
-        <v>84.0</v>
+        <v>26.0</v>
       </c>
       <c r="F6" t="n">
-        <v>3.96357880596532E-5</v>
+        <v>0.00799712708568516</v>
       </c>
       <c r="G6" t="n">
-        <v>1.4175710770138E-6</v>
+        <v>4.03810600803007E-5</v>
       </c>
       <c r="H6" t="n">
-        <v>8.72881864945047E-5</v>
+        <v>1.22060965342091E-9</v>
       </c>
       <c r="I6" t="n">
-        <v>80.0</v>
+        <v>70.0</v>
       </c>
       <c r="J6" t="n">
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1784355179704017</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0026742305794235717</v>
+        <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N6" t="n">
         <v>0.0</v>
@@ -3167,43 +3167,43 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="D7" t="n">
+        <v>158.0</v>
+      </c>
+      <c r="E7" t="n">
         <v>46.0</v>
       </c>
-      <c r="E7" t="n">
-        <v>19.0</v>
-      </c>
       <c r="F7" t="n">
-        <v>3.98211137138711E-5</v>
+        <v>3.96357880596532E-5</v>
       </c>
       <c r="G7" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00625718664081437</v>
+        <v>0.00152282025112865</v>
       </c>
       <c r="I7" t="n">
-        <v>70.0</v>
+        <v>60.0</v>
       </c>
       <c r="J7" t="n">
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.040169133192389</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L7" t="n">
         <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -3211,43 +3211,43 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
         <v>84</v>
       </c>
       <c r="D8" t="n">
-        <v>265.0</v>
+        <v>46.0</v>
       </c>
       <c r="E8" t="n">
-        <v>34.0</v>
+        <v>19.0</v>
       </c>
       <c r="F8" t="n">
-        <v>4.03810600803007E-5</v>
+        <v>3.98211137138711E-5</v>
       </c>
       <c r="G8" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H8" t="n">
-        <v>5.41340370300314E-5</v>
+        <v>0.00625718664081437</v>
       </c>
       <c r="I8" t="n">
-        <v>70.0</v>
+        <v>50.0</v>
       </c>
       <c r="J8" t="n">
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N8" t="n">
         <v>0.0</v>
@@ -3255,28 +3255,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" t="n">
-        <v>103.0</v>
+        <v>265.0</v>
       </c>
       <c r="E9" t="n">
-        <v>19.0</v>
+        <v>34.0</v>
       </c>
       <c r="F9" t="n">
-        <v>3.98211137138711E-5</v>
+        <v>4.03810600803007E-5</v>
       </c>
       <c r="G9" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H9" t="n">
-        <v>4.20631113667766E-4</v>
+        <v>5.41340370300314E-5</v>
       </c>
       <c r="I9" t="n">
         <v>50.0</v>
@@ -3285,13 +3285,13 @@
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.040169133192389</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -3299,28 +3299,28 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" t="n">
-        <v>29.0</v>
+        <v>48.0</v>
       </c>
       <c r="E10" t="n">
-        <v>26.0</v>
+        <v>15.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00799712708568516</v>
+        <v>3.83568771824305E-5</v>
       </c>
       <c r="G10" t="n">
-        <v>4.03810600803007E-5</v>
+        <v>1.4175710770138E-6</v>
       </c>
       <c r="H10" t="n">
-        <v>1.22060965342091E-9</v>
+        <v>0.00180163808571658</v>
       </c>
       <c r="I10" t="n">
         <v>50.0</v>
@@ -3329,13 +3329,13 @@
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -3343,43 +3343,43 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D11" t="n">
-        <v>250.0</v>
+        <v>158.0</v>
       </c>
       <c r="E11" t="n">
-        <v>26.0</v>
+        <v>84.0</v>
       </c>
       <c r="F11" t="n">
-        <v>3.98211137138711E-5</v>
+        <v>3.96357880596532E-5</v>
       </c>
       <c r="G11" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00470560456401602</v>
+        <v>8.72881864945047E-5</v>
       </c>
       <c r="I11" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
       <c r="J11" t="n">
         <v>100.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.17864693446088797</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0</v>
+        <v>0.002283559090348079</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N11" t="n">
         <v>0.0</v>
@@ -3387,31 +3387,31 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
         <v>87</v>
       </c>
       <c r="D12" t="n">
-        <v>48.0</v>
+        <v>103.0</v>
       </c>
       <c r="E12" t="n">
         <v>15.0</v>
       </c>
       <c r="F12" t="n">
-        <v>3.83568771824305E-5</v>
+        <v>3.96357880596532E-5</v>
       </c>
       <c r="G12" t="n">
-        <v>1.4175710770138E-6</v>
+        <v>9.05702480294115E-5</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00180163808571658</v>
+        <v>0.00920956456293582</v>
       </c>
       <c r="I12" t="n">
-        <v>40.0</v>
+        <v>30.0</v>
       </c>
       <c r="J12" t="n">
         <v>100.0</v>
@@ -3431,72 +3431,72 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D13" t="n">
-        <v>32.0</v>
+        <v>250.0</v>
       </c>
       <c r="E13" t="n">
-        <v>2.0</v>
+        <v>26.0</v>
       </c>
       <c r="F13" t="n">
-        <v>3.64111620331533E-5</v>
+        <v>3.98211137138711E-5</v>
       </c>
       <c r="G13" t="n">
-        <v>3.14719354078108E-5</v>
+        <v>1.4175710770138E-6</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00389687175260687</v>
+        <v>0.00470560456401602</v>
       </c>
       <c r="I13" t="n">
-        <v>40.0</v>
+        <v>30.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.004228329809725159</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M13" t="n">
-        <v>0.00422832980972516</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D14" t="n">
-        <v>141.0</v>
+        <v>93.0</v>
       </c>
       <c r="E14" t="n">
-        <v>34.0</v>
+        <v>84.0</v>
       </c>
       <c r="F14" t="n">
-        <v>4.01937482104294E-5</v>
+        <v>0.00260366851725413</v>
       </c>
       <c r="G14" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H14" t="n">
-        <v>0.00103577594631515</v>
+        <v>2.66335709542836E-4</v>
       </c>
       <c r="I14" t="n">
         <v>30.0</v>
@@ -3505,13 +3505,13 @@
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.17864693446088797</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0</v>
+        <v>0.002283559090348079</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N14" t="n">
         <v>0.0</v>
@@ -3525,22 +3525,22 @@
         <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="D15" t="n">
-        <v>93.0</v>
+        <v>32.0</v>
       </c>
       <c r="E15" t="n">
-        <v>84.0</v>
+        <v>2.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00260366851725413</v>
+        <v>3.64111620331533E-5</v>
       </c>
       <c r="G15" t="n">
-        <v>1.4175710770138E-6</v>
+        <v>3.14719354078108E-5</v>
       </c>
       <c r="H15" t="n">
-        <v>2.66335709542836E-4</v>
+        <v>0.00389687175260687</v>
       </c>
       <c r="I15" t="n">
         <v>30.0</v>
@@ -3549,13 +3549,13 @@
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1784355179704017</v>
+        <v>0.004228329809725159</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0026742305794235717</v>
+        <v>0.0</v>
       </c>
       <c r="M15" t="n">
-        <v>0.177589852008457</v>
+        <v>0.00422832980972516</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -3563,28 +3563,28 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D16" t="n">
-        <v>120.0</v>
+        <v>103.0</v>
       </c>
       <c r="E16" t="n">
-        <v>82.0</v>
+        <v>19.0</v>
       </c>
       <c r="F16" t="n">
-        <v>3.94511214512808E-5</v>
+        <v>3.98211137138711E-5</v>
       </c>
       <c r="G16" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00112197360386636</v>
+        <v>4.20631113667766E-4</v>
       </c>
       <c r="I16" t="n">
         <v>20.0</v>
@@ -3593,13 +3593,13 @@
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L16" t="n">
         <v>0.0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.173361522198731</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -3607,28 +3607,28 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
         <v>90</v>
       </c>
       <c r="D17" t="n">
-        <v>26.0</v>
+        <v>120.0</v>
       </c>
       <c r="E17" t="n">
-        <v>25.0</v>
+        <v>82.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.152526861987935</v>
+        <v>3.94511214512808E-5</v>
       </c>
       <c r="G17" t="n">
-        <v>5.32401707922167E-5</v>
+        <v>1.4175710770138E-6</v>
       </c>
       <c r="H17" t="n">
-        <v>4.94689940303263E-4</v>
+        <v>0.00112197360386636</v>
       </c>
       <c r="I17" t="n">
         <v>20.0</v>
@@ -3637,13 +3637,13 @@
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -3651,28 +3651,28 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
       </c>
       <c r="D18" t="n">
-        <v>265.0</v>
+        <v>26.0</v>
       </c>
       <c r="E18" t="n">
-        <v>23.0</v>
+        <v>25.0</v>
       </c>
       <c r="F18" t="n">
-        <v>4.00070999263567E-5</v>
+        <v>0.152526861987935</v>
       </c>
       <c r="G18" t="n">
-        <v>4.05690370510693E-5</v>
+        <v>5.32401707922167E-5</v>
       </c>
       <c r="H18" t="n">
-        <v>2.49022843057501E-4</v>
+        <v>4.94689940303263E-4</v>
       </c>
       <c r="I18" t="n">
         <v>20.0</v>
@@ -3681,13 +3681,13 @@
         <v>100.0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L18" t="n">
         <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N18" t="n">
         <v>0.0</v>
@@ -3695,43 +3695,43 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D19" t="n">
-        <v>48.0</v>
+        <v>265.0</v>
       </c>
       <c r="E19" t="n">
-        <v>19.0</v>
+        <v>23.0</v>
       </c>
       <c r="F19" t="n">
-        <v>3.98211137138711E-5</v>
+        <v>4.00070999263567E-5</v>
       </c>
       <c r="G19" t="n">
-        <v>4.03810600803007E-5</v>
+        <v>4.05690370510693E-5</v>
       </c>
       <c r="H19" t="n">
-        <v>0.00205785005792113</v>
+        <v>2.49022843057501E-4</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.040169133192389</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L19" t="n">
         <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N19" t="n">
         <v>0.0</v>
@@ -3739,28 +3739,28 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D20" t="n">
-        <v>250.0</v>
+        <v>48.0</v>
       </c>
       <c r="E20" t="n">
-        <v>27.0</v>
+        <v>19.0</v>
       </c>
       <c r="F20" t="n">
+        <v>3.98211137138711E-5</v>
+      </c>
+      <c r="G20" t="n">
         <v>4.03810600803007E-5</v>
       </c>
-      <c r="G20" t="n">
-        <v>1.4175710770138E-6</v>
-      </c>
       <c r="H20" t="n">
-        <v>0.0156710438786786</v>
+        <v>0.00205785005792113</v>
       </c>
       <c r="I20" t="n">
         <v>0.0</v>
@@ -3769,42 +3769,42 @@
         <v>0.0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.05708245243128964</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L20" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0570824524312896</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N20" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D21" t="n">
-        <v>266.0</v>
+        <v>250.0</v>
       </c>
       <c r="E21" t="n">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="F21" t="n">
-        <v>3.94511214512808E-5</v>
+        <v>4.03810600803007E-5</v>
       </c>
       <c r="G21" t="n">
         <v>1.4175710770138E-6</v>
       </c>
       <c r="H21" t="n">
-        <v>6.07025207439655E-5</v>
+        <v>0.0156710438786786</v>
       </c>
       <c r="I21" t="n">
         <v>0.0</v>
@@ -3813,13 +3813,13 @@
         <v>0.0</v>
       </c>
       <c r="K21" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.05708245243128964</v>
       </c>
       <c r="L21" t="n">
         <v>0.0</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0570824524312896</v>
       </c>
       <c r="N21" t="n">
         <v>2.31296463463574E-18</v>
@@ -3827,28 +3827,28 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D22" t="n">
-        <v>250.0</v>
+        <v>266.0</v>
       </c>
       <c r="E22" t="n">
-        <v>34.0</v>
+        <v>28.0</v>
       </c>
       <c r="F22" t="n">
-        <v>4.05690370510693E-5</v>
+        <v>3.94511214512808E-5</v>
       </c>
       <c r="G22" t="n">
-        <v>2.8351421540276E-6</v>
+        <v>1.4175710770138E-6</v>
       </c>
       <c r="H22" t="n">
-        <v>0.00966219049106077</v>
+        <v>6.07025207439655E-5</v>
       </c>
       <c r="I22" t="n">
         <v>0.0</v>
@@ -3857,13 +3857,13 @@
         <v>0.0</v>
       </c>
       <c r="K22" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L22" t="n">
         <v>0.0</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N22" t="n">
         <v>0.0</v>
@@ -3871,28 +3871,28 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D23" t="n">
-        <v>27.0</v>
+        <v>250.0</v>
       </c>
       <c r="E23" t="n">
-        <v>15.0</v>
+        <v>34.0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.91206465349113E-4</v>
+        <v>4.05690370510693E-5</v>
       </c>
       <c r="G23" t="n">
-        <v>2.76426360017691E-4</v>
+        <v>2.8351421540276E-6</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0262910800339557</v>
+        <v>0.00966219049106077</v>
       </c>
       <c r="I23" t="n">
         <v>0.0</v>
@@ -3901,13 +3901,13 @@
         <v>0.0</v>
       </c>
       <c r="K23" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L23" t="n">
         <v>0.0</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N23" t="n">
         <v>0.0</v>
@@ -3915,28 +3915,28 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D24" t="n">
-        <v>250.0</v>
+        <v>27.0</v>
       </c>
       <c r="E24" t="n">
         <v>15.0</v>
       </c>
       <c r="F24" t="n">
-        <v>4.00070999263567E-5</v>
+        <v>1.91206465349113E-4</v>
       </c>
       <c r="G24" t="n">
-        <v>4.05690370510693E-5</v>
+        <v>2.76426360017691E-4</v>
       </c>
       <c r="H24" t="n">
-        <v>0.00325805922031213</v>
+        <v>0.0262910800339557</v>
       </c>
       <c r="I24" t="n">
         <v>0.0</v>
@@ -3959,34 +3959,34 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D25" t="n">
-        <v>103.0</v>
+        <v>250.0</v>
       </c>
       <c r="E25" t="n">
         <v>15.0</v>
       </c>
       <c r="F25" t="n">
-        <v>3.96357880596532E-5</v>
+        <v>4.00070999263567E-5</v>
       </c>
       <c r="G25" t="n">
-        <v>9.05702480294115E-5</v>
+        <v>4.05690370510693E-5</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00920956456293582</v>
+        <v>0.00325805922031213</v>
       </c>
       <c r="I25" t="n">
         <v>0.0</v>
       </c>
       <c r="J25" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K25" t="n">
         <v>0.03171247357293869</v>
@@ -4006,7 +4006,7 @@
         <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
         <v>94</v>
@@ -4036,7 +4036,7 @@
         <v>0.12473572938689217</v>
       </c>
       <c r="L26" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M26" t="n">
         <v>0.124735729386892</v>
@@ -4047,10 +4047,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
         <v>94</v>
@@ -4080,7 +4080,7 @@
         <v>0.12473572938689217</v>
       </c>
       <c r="L27" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M27" t="n">
         <v>0.124735729386892</v>
@@ -4091,7 +4091,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
         <v>68</v>
@@ -4138,7 +4138,7 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
         <v>96</v>
@@ -4168,13 +4168,13 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L29" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M29" t="n">
         <v>0.0591966173361522</v>
       </c>
       <c r="N29" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="30">
@@ -4185,7 +4185,7 @@
         <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D30" t="n">
         <v>31.0</v>
@@ -4218,7 +4218,7 @@
         <v>0.0528541226215645</v>
       </c>
       <c r="N30" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
@@ -4229,7 +4229,7 @@
         <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31" t="n">
         <v>64.0</v>
@@ -4273,7 +4273,7 @@
         <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D32" t="n">
         <v>120.0</v>
@@ -4314,10 +4314,10 @@
         <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D33" t="n">
         <v>84.0</v>
@@ -4361,7 +4361,7 @@
         <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D34" t="n">
         <v>28.0</v>
@@ -4388,7 +4388,7 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M34" t="n">
         <v>0.0528541226215645</v>
@@ -4405,7 +4405,7 @@
         <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D35" t="n">
         <v>41.0</v>
@@ -4432,7 +4432,7 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L35" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M35" t="n">
         <v>0.0528541226215645</v>
@@ -4443,13 +4443,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
         <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D36" t="n">
         <v>31.0</v>
@@ -4476,21 +4476,21 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L36" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M36" t="n">
         <v>0.0528541226215645</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
         <v>99</v>
@@ -4534,7 +4534,7 @@
         <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
         <v>100</v>
@@ -4564,21 +4564,21 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L38" t="n">
-        <v>8.012344526598183E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M38" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N38" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s">
         <v>101</v>
@@ -4622,10 +4622,10 @@
         <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D40" t="n">
         <v>26.0</v>
@@ -4666,10 +4666,10 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D41" t="n">
         <v>25.0</v>
@@ -4740,13 +4740,13 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L42" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M42" t="n">
         <v>0.0570824524312896</v>
       </c>
       <c r="N42" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="43">
@@ -4784,7 +4784,7 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L43" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M43" t="n">
         <v>0.0570824524312896</v>
@@ -4828,7 +4828,7 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L44" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M44" t="n">
         <v>0.06553911205074</v>
@@ -4872,13 +4872,13 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L45" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M45" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N45" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="46">
@@ -4930,10 +4930,10 @@
         <v>60</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D47" t="n">
         <v>46.0</v>
@@ -4974,10 +4974,10 @@
         <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D48" t="n">
         <v>93.0</v>
@@ -5018,7 +5018,7 @@
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
         <v>78</v>
@@ -5048,7 +5048,7 @@
         <v>0.05496828752642706</v>
       </c>
       <c r="L49" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M49" t="n">
         <v>0.0549682875264271</v>
@@ -5092,7 +5092,7 @@
         <v>0.05496828752642706</v>
       </c>
       <c r="L50" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M50" t="n">
         <v>0.0549682875264271</v>
@@ -5150,7 +5150,7 @@
         <v>133</v>
       </c>
       <c r="B52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C52" t="s">
         <v>73</v>
@@ -5241,7 +5241,7 @@
         <v>68</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D54" t="n">
         <v>250.0</v>
@@ -5417,7 +5417,7 @@
         <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D58" t="e">
         <v>#NUM!</v>
@@ -5461,7 +5461,7 @@
         <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D59" t="e">
         <v>#NUM!</v>
@@ -5543,7 +5543,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
         <v>79</v>
@@ -5637,7 +5637,7 @@
         <v>79</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D63" t="e">
         <v>#NUM!</v>
@@ -5675,13 +5675,13 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
         <v>79</v>
       </c>
       <c r="C64" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D64" t="e">
         <v>#NUM!</v>
@@ -5857,7 +5857,7 @@
         <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D68" t="e">
         <v>#NUM!</v>
@@ -5925,10 +5925,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K69" t="n">
-        <v>0.48773784355179706</v>
+        <v>0.48520084566596194</v>
       </c>
       <c r="L69" t="n">
-        <v>0.0067631250818943524</v>
+        <v>0.003342788224279473</v>
       </c>
       <c r="M69" t="e">
         <v>#NUM!</v>
@@ -6033,7 +6033,7 @@
         <v>79</v>
       </c>
       <c r="C72" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D72" t="e">
         <v>#NUM!</v>

</xml_diff>

<commit_message>
added some comments in first part of the project
</commit_message>
<xml_diff>
--- a/output/LUAD_statistics_.xlsx
+++ b/output/LUAD_statistics_.xlsx
@@ -54,60 +54,60 @@
     <t>capri_bic.SD.POSTERR</t>
   </si>
   <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
-    <t>6</t>
+    <t>8</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>8</t>
+    <t>27</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>31</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>32</t>
   </si>
   <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>19</t>
+    <t>10</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -216,75 +216,75 @@
     <t>54</t>
   </si>
   <si>
+    <t>Mutation TP53</t>
+  </si>
+  <si>
+    <t>Pattern OR_CDK4_TP53</t>
+  </si>
+  <si>
+    <t>Pattern OR_KRAS</t>
+  </si>
+  <si>
+    <t>Mutation ATM</t>
+  </si>
+  <si>
     <t>Mutation EGFR</t>
   </si>
   <si>
-    <t>Pattern OR_CDK4_TP53</t>
-  </si>
-  <si>
-    <t>Pattern OR_KRAS</t>
-  </si>
-  <si>
-    <t>Mutation TP53</t>
-  </si>
-  <si>
-    <t>Mutation ATM</t>
+    <t>Mutation SMARCA4</t>
   </si>
   <si>
     <t>Amplification CDK4</t>
   </si>
   <si>
-    <t>Mutation SMARCA4</t>
+    <t>Pattern OR_CDKN2A</t>
+  </si>
+  <si>
+    <t>Mutation ROS1</t>
+  </si>
+  <si>
+    <t>Mutation KEAP1</t>
   </si>
   <si>
     <t>Mutation KRAS</t>
   </si>
   <si>
-    <t>Pattern OR_CDKN2A</t>
-  </si>
-  <si>
-    <t>Mutation KEAP1</t>
-  </si>
-  <si>
-    <t>Mutation ROS1</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
+    <t>Mutation RB1</t>
+  </si>
+  <si>
     <t>Amplification EGFR</t>
   </si>
   <si>
-    <t>Mutation RB1</t>
+    <t>Mutation STK11</t>
   </si>
   <si>
     <t>Amplification CCND1</t>
   </si>
   <si>
-    <t>Mutation STK11</t>
-  </si>
-  <si>
     <t>Amplification KRAS</t>
   </si>
   <si>
+    <t>Mutation NFE2L2</t>
+  </si>
+  <si>
     <t>Amplification MDM2</t>
   </si>
   <si>
-    <t>Mutation NFE2L2</t>
-  </si>
-  <si>
     <t>Mutation RET</t>
   </si>
   <si>
+    <t>Mutation ARID1B</t>
+  </si>
+  <si>
     <t>Mutation CDKN2A</t>
   </si>
   <si>
     <t>Amplification MET</t>
   </si>
   <si>
-    <t>Mutation ARID1B</t>
-  </si>
-  <si>
     <t>Amplification CCNE1</t>
   </si>
   <si>
@@ -414,10 +414,10 @@
     <t>55</t>
   </si>
   <si>
+    <t>59</t>
+  </si>
+  <si>
     <t>58</t>
-  </si>
-  <si>
-    <t>59</t>
   </si>
   <si>
     <t>56</t>
@@ -584,34 +584,34 @@
         <v>79</v>
       </c>
       <c r="D2" t="n">
-        <v>65.0</v>
+        <v>250.0</v>
       </c>
       <c r="E2" t="n">
-        <v>28.0</v>
+        <v>31.0</v>
       </c>
       <c r="F2" t="n">
-        <v>8.78077655229543E-5</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G2" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H2" t="n">
-        <v>5.79183644388044E-8</v>
+        <v>1.26016181125199E-5</v>
       </c>
       <c r="I2" t="n">
-        <v>90.0</v>
+        <v>100.0</v>
       </c>
       <c r="J2" t="n">
         <v>100.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L2" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>6.542051911182396E-18</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N2" t="n">
         <v>0.0</v>
@@ -625,7 +625,7 @@
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" t="n">
         <v>265.0</v>
@@ -652,13 +652,13 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L3" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M3" t="n">
         <v>0.0591966173361522</v>
       </c>
       <c r="N3" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -669,13 +669,13 @@
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D4" t="n">
         <v>158.0</v>
       </c>
       <c r="E4" t="n">
-        <v>46.0</v>
+        <v>84.0</v>
       </c>
       <c r="F4" t="n">
         <v>8.83055058344676E-5</v>
@@ -684,7 +684,7 @@
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00136380139658682</v>
+        <v>1.06490214720269E-4</v>
       </c>
       <c r="I4" t="n">
         <v>90.0</v>
@@ -693,13 +693,13 @@
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.17885835095137423</v>
       </c>
       <c r="L4" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.004011345869135358</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N4" t="n">
         <v>0.0</v>
@@ -713,40 +713,40 @@
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D5" t="n">
-        <v>250.0</v>
+        <v>46.0</v>
       </c>
       <c r="E5" t="n">
-        <v>31.0</v>
+        <v>19.0</v>
       </c>
       <c r="F5" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>8.9307244186841E-5</v>
       </c>
       <c r="G5" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H5" t="n">
-        <v>1.26016181125199E-5</v>
+        <v>0.00107415299691177</v>
       </c>
       <c r="I5" t="n">
-        <v>90.0</v>
+        <v>80.0</v>
       </c>
       <c r="J5" t="n">
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L5" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.06553911205074</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N5" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -757,22 +757,22 @@
         <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" t="n">
-        <v>46.0</v>
+        <v>65.0</v>
       </c>
       <c r="E6" t="n">
-        <v>19.0</v>
+        <v>28.0</v>
       </c>
       <c r="F6" t="n">
-        <v>8.9307244186841E-5</v>
+        <v>8.78077655229543E-5</v>
       </c>
       <c r="G6" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00107415299691177</v>
+        <v>5.79183644388044E-8</v>
       </c>
       <c r="I6" t="n">
         <v>80.0</v>
@@ -781,13 +781,13 @@
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.041014799154334036</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0026742305794235782</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M6" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N6" t="n">
         <v>0.0</v>
@@ -798,25 +798,25 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D7" t="n">
-        <v>158.0</v>
+        <v>265.0</v>
       </c>
       <c r="E7" t="n">
-        <v>84.0</v>
+        <v>34.0</v>
       </c>
       <c r="F7" t="n">
-        <v>8.83055058344676E-5</v>
+        <v>9.08255730457327E-5</v>
       </c>
       <c r="G7" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H7" t="n">
-        <v>1.06490214720269E-4</v>
+        <v>1.52049237002162E-5</v>
       </c>
       <c r="I7" t="n">
         <v>80.0</v>
@@ -825,13 +825,13 @@
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.17801268498942918</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0013371152897117859</v>
+        <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -842,40 +842,40 @@
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D8" t="n">
-        <v>265.0</v>
+        <v>158.0</v>
       </c>
       <c r="E8" t="n">
-        <v>34.0</v>
+        <v>46.0</v>
       </c>
       <c r="F8" t="n">
-        <v>9.08255730457327E-5</v>
+        <v>8.83055058344676E-5</v>
       </c>
       <c r="G8" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H8" t="n">
-        <v>1.52049237002162E-5</v>
+        <v>0.00136380139658682</v>
       </c>
       <c r="I8" t="n">
-        <v>50.0</v>
+        <v>80.0</v>
       </c>
       <c r="J8" t="n">
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N8" t="n">
         <v>0.0</v>
@@ -892,34 +892,34 @@
         <v>84</v>
       </c>
       <c r="D9" t="n">
-        <v>29.0</v>
+        <v>48.0</v>
       </c>
       <c r="E9" t="n">
-        <v>26.0</v>
+        <v>15.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0030724418147686</v>
+        <v>8.78077655229543E-5</v>
       </c>
       <c r="G9" t="n">
-        <v>9.03173604037676E-5</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H9" t="n">
-        <v>1.39310535932318E-8</v>
+        <v>0.00180163808571658</v>
       </c>
       <c r="I9" t="n">
-        <v>50.0</v>
+        <v>70.0</v>
       </c>
       <c r="J9" t="n">
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -936,19 +936,19 @@
         <v>85</v>
       </c>
       <c r="D10" t="n">
-        <v>48.0</v>
+        <v>29.0</v>
       </c>
       <c r="E10" t="n">
-        <v>15.0</v>
+        <v>26.0</v>
       </c>
       <c r="F10" t="n">
-        <v>8.78077655229543E-5</v>
+        <v>0.0030724418147686</v>
       </c>
       <c r="G10" t="n">
-        <v>5.41254411223451E-6</v>
+        <v>9.03173604037676E-5</v>
       </c>
       <c r="H10" t="n">
-        <v>0.00180163808571658</v>
+        <v>1.39310535932318E-8</v>
       </c>
       <c r="I10" t="n">
         <v>50.0</v>
@@ -957,13 +957,13 @@
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -995,7 +995,7 @@
         <v>4.17481529274546E-4</v>
       </c>
       <c r="I11" t="n">
-        <v>40.0</v>
+        <v>50.0</v>
       </c>
       <c r="J11" t="n">
         <v>100.0</v>
@@ -1018,25 +1018,25 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D12" t="n">
-        <v>250.0</v>
+        <v>103.0</v>
       </c>
       <c r="E12" t="n">
-        <v>26.0</v>
+        <v>19.0</v>
       </c>
       <c r="F12" t="n">
-        <v>8.8805330344482E-5</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G12" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00184132981093954</v>
+        <v>6.66551822225193E-5</v>
       </c>
       <c r="I12" t="n">
         <v>40.0</v>
@@ -1045,16 +1045,16 @@
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N12" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -1062,43 +1062,43 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D13" t="n">
-        <v>141.0</v>
+        <v>26.0</v>
       </c>
       <c r="E13" t="n">
-        <v>34.0</v>
+        <v>25.0</v>
       </c>
       <c r="F13" t="n">
-        <v>9.03173604037676E-5</v>
+        <v>0.234147355744326</v>
       </c>
       <c r="G13" t="n">
-        <v>5.41254411223451E-6</v>
+        <v>1.22402412262228E-4</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00187504170433014</v>
+        <v>3.8759431457377E-4</v>
       </c>
       <c r="I13" t="n">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="14">
@@ -1106,25 +1106,25 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D14" t="n">
-        <v>103.0</v>
+        <v>250.0</v>
       </c>
       <c r="E14" t="n">
-        <v>19.0</v>
+        <v>25.0</v>
       </c>
       <c r="F14" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>9.03173604037676E-5</v>
       </c>
       <c r="G14" t="n">
-        <v>5.41254411223451E-6</v>
+        <v>3.78878087856416E-5</v>
       </c>
       <c r="H14" t="n">
-        <v>6.66551822225193E-5</v>
+        <v>0.00184132981093954</v>
       </c>
       <c r="I14" t="n">
         <v>20.0</v>
@@ -1133,16 +1133,16 @@
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.041014799154334036</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0026742305794235782</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M14" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="15">
@@ -1150,22 +1150,22 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D15" t="n">
         <v>250.0</v>
       </c>
       <c r="E15" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="F15" t="n">
-        <v>9.03173604037676E-5</v>
+        <v>8.8805330344482E-5</v>
       </c>
       <c r="G15" t="n">
-        <v>3.78878087856416E-5</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H15" t="n">
         <v>0.00184132981093954</v>
@@ -1177,13 +1177,13 @@
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -1194,25 +1194,25 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D16" t="n">
-        <v>103.0</v>
+        <v>93.0</v>
       </c>
       <c r="E16" t="n">
-        <v>48.0</v>
+        <v>84.0</v>
       </c>
       <c r="F16" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>0.00770455162977997</v>
       </c>
       <c r="G16" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00159648799018954</v>
+        <v>3.42756749960878E-4</v>
       </c>
       <c r="I16" t="n">
         <v>20.0</v>
@@ -1221,13 +1221,13 @@
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1014799154334038</v>
+        <v>0.17885835095137423</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0</v>
+        <v>0.004011345869135358</v>
       </c>
       <c r="M16" t="n">
-        <v>0.101479915433404</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -1238,40 +1238,40 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D17" t="n">
-        <v>93.0</v>
+        <v>141.0</v>
       </c>
       <c r="E17" t="n">
-        <v>84.0</v>
+        <v>34.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00770455162977997</v>
+        <v>9.03173604037676E-5</v>
       </c>
       <c r="G17" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H17" t="n">
-        <v>3.42756749960878E-4</v>
+        <v>0.00187504170433014</v>
       </c>
       <c r="I17" t="n">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
       <c r="J17" t="n">
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.17801268498942918</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0013371152897117859</v>
+        <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -1282,10 +1282,10 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D18" t="n">
         <v>103.0</v>
@@ -1326,40 +1326,40 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="D19" t="n">
-        <v>26.0</v>
+        <v>103.0</v>
       </c>
       <c r="E19" t="n">
-        <v>25.0</v>
+        <v>48.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.234147355744326</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G19" t="n">
-        <v>1.22402412262228E-4</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H19" t="n">
-        <v>3.8759431457377E-4</v>
+        <v>0.00159648799018954</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="J19" t="n">
         <v>100.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.1014799154334038</v>
       </c>
       <c r="L19" t="n">
         <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.101479915433404</v>
       </c>
       <c r="N19" t="n">
         <v>0.0</v>
@@ -1400,7 +1400,7 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M20" t="e">
         <v>#NUM!</v>
@@ -1417,7 +1417,7 @@
         <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D21" t="e">
         <v>#NUM!</v>
@@ -1444,7 +1444,7 @@
         <v>0.0613107822410148</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M21" t="e">
         <v>#NUM!</v>
@@ -1620,7 +1620,7 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L25" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M25" t="e">
         <v>#NUM!</v>
@@ -1664,7 +1664,7 @@
         <v>0.06765327695560254</v>
       </c>
       <c r="L26" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M26" t="e">
         <v>#NUM!</v>
@@ -1725,7 +1725,7 @@
         <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D28" t="e">
         <v>#NUM!</v>
@@ -1857,7 +1857,7 @@
         <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D31" t="e">
         <v>#NUM!</v>
@@ -1928,7 +1928,7 @@
         <v>0.04439746300211417</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M32" t="e">
         <v>#NUM!</v>
@@ -1972,7 +1972,7 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L33" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M33" t="e">
         <v>#NUM!</v>
@@ -2016,7 +2016,7 @@
         <v>0.13530655391120508</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0</v>
+        <v>9.25185853854297E-18</v>
       </c>
       <c r="M34" t="e">
         <v>#NUM!</v>
@@ -2165,7 +2165,7 @@
         <v>78</v>
       </c>
       <c r="C38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D38" t="e">
         <v>#NUM!</v>
@@ -2341,7 +2341,7 @@
         <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D42" t="e">
         <v>#NUM!</v>
@@ -2453,10 +2453,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K44" t="n">
-        <v>0.4945031712473573</v>
+        <v>0.48477801268498943</v>
       </c>
       <c r="L44" t="n">
-        <v>0.015709128886722563</v>
+        <v>0.0020056729345676876</v>
       </c>
       <c r="M44" t="e">
         <v>#NUM!</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>67</v>
@@ -3015,48 +3015,48 @@
         <v>79</v>
       </c>
       <c r="D2" t="n">
-        <v>65.0</v>
+        <v>250.0</v>
       </c>
       <c r="E2" t="n">
-        <v>28.0</v>
+        <v>31.0</v>
       </c>
       <c r="F2" t="n">
-        <v>8.78077655229543E-5</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G2" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H2" t="n">
-        <v>5.79183644388044E-8</v>
+        <v>1.26016181125199E-5</v>
       </c>
       <c r="I2" t="n">
-        <v>90.0</v>
+        <v>100.0</v>
       </c>
       <c r="J2" t="n">
         <v>100.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.06553911205073996</v>
       </c>
       <c r="L2" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>6.542051911182396E-18</v>
       </c>
       <c r="M2" t="n">
-        <v>0.125581395348837</v>
+        <v>0.06553911205074</v>
       </c>
       <c r="N2" t="n">
-        <v>0.00447928078423417</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" t="n">
         <v>265.0</v>
@@ -3083,30 +3083,30 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L3" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M3" t="n">
         <v>0.0591966173361522</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D4" t="n">
         <v>158.0</v>
       </c>
       <c r="E4" t="n">
-        <v>46.0</v>
+        <v>84.0</v>
       </c>
       <c r="F4" t="n">
         <v>8.83055058344676E-5</v>
@@ -3115,7 +3115,7 @@
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H4" t="n">
-        <v>0.00136380139658682</v>
+        <v>1.06490214720269E-4</v>
       </c>
       <c r="I4" t="n">
         <v>90.0</v>
@@ -3124,13 +3124,13 @@
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.17885835095137423</v>
       </c>
       <c r="L4" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.004011345869135358</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N4" t="n">
         <v>0.0</v>
@@ -3138,43 +3138,43 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D5" t="n">
-        <v>250.0</v>
+        <v>46.0</v>
       </c>
       <c r="E5" t="n">
-        <v>31.0</v>
+        <v>19.0</v>
       </c>
       <c r="F5" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>8.9307244186841E-5</v>
       </c>
       <c r="G5" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H5" t="n">
-        <v>1.26016181125199E-5</v>
+        <v>0.00107415299691177</v>
       </c>
       <c r="I5" t="n">
-        <v>90.0</v>
+        <v>80.0</v>
       </c>
       <c r="J5" t="n">
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.06553911205073996</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L5" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.06553911205074</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N5" t="n">
         <v>0.0</v>
@@ -3182,28 +3182,28 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" t="n">
-        <v>46.0</v>
+        <v>65.0</v>
       </c>
       <c r="E6" t="n">
-        <v>19.0</v>
+        <v>28.0</v>
       </c>
       <c r="F6" t="n">
-        <v>8.9307244186841E-5</v>
+        <v>8.78077655229543E-5</v>
       </c>
       <c r="G6" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H6" t="n">
-        <v>0.00107415299691177</v>
+        <v>5.79183644388044E-8</v>
       </c>
       <c r="I6" t="n">
         <v>80.0</v>
@@ -3212,42 +3212,42 @@
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.041014799154334036</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0026742305794235782</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M6" t="n">
-        <v>0.040169133192389</v>
+        <v>0.120718816067653</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0</v>
+        <v>0.00365505355317546</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D7" t="n">
-        <v>158.0</v>
+        <v>265.0</v>
       </c>
       <c r="E7" t="n">
-        <v>84.0</v>
+        <v>34.0</v>
       </c>
       <c r="F7" t="n">
-        <v>8.83055058344676E-5</v>
+        <v>9.08255730457327E-5</v>
       </c>
       <c r="G7" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H7" t="n">
-        <v>1.06490214720269E-4</v>
+        <v>1.52049237002162E-5</v>
       </c>
       <c r="I7" t="n">
         <v>80.0</v>
@@ -3256,13 +3256,13 @@
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.17801268498942918</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0013371152897117859</v>
+        <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -3270,43 +3270,43 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D8" t="n">
-        <v>265.0</v>
+        <v>158.0</v>
       </c>
       <c r="E8" t="n">
-        <v>34.0</v>
+        <v>46.0</v>
       </c>
       <c r="F8" t="n">
-        <v>9.08255730457327E-5</v>
+        <v>8.83055058344676E-5</v>
       </c>
       <c r="G8" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H8" t="n">
-        <v>1.52049237002162E-5</v>
+        <v>0.00136380139658682</v>
       </c>
       <c r="I8" t="n">
-        <v>50.0</v>
+        <v>80.0</v>
       </c>
       <c r="J8" t="n">
         <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L8" t="n">
         <v>0.0</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N8" t="n">
         <v>0.0</v>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
         <v>72</v>
@@ -3323,42 +3323,42 @@
         <v>84</v>
       </c>
       <c r="D9" t="n">
-        <v>29.0</v>
+        <v>48.0</v>
       </c>
       <c r="E9" t="n">
-        <v>26.0</v>
+        <v>15.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0030724418147686</v>
+        <v>8.78077655229543E-5</v>
       </c>
       <c r="G9" t="n">
-        <v>9.03173604037676E-5</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H9" t="n">
-        <v>1.39310535932318E-8</v>
+        <v>0.00180163808571658</v>
       </c>
       <c r="I9" t="n">
-        <v>50.0</v>
+        <v>70.0</v>
       </c>
       <c r="J9" t="n">
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0553911205073996</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N9" t="n">
-        <v>0.00133711528971179</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
         <v>73</v>
@@ -3367,19 +3367,19 @@
         <v>85</v>
       </c>
       <c r="D10" t="n">
-        <v>48.0</v>
+        <v>29.0</v>
       </c>
       <c r="E10" t="n">
-        <v>15.0</v>
+        <v>26.0</v>
       </c>
       <c r="F10" t="n">
-        <v>8.78077655229543E-5</v>
+        <v>0.0030724418147686</v>
       </c>
       <c r="G10" t="n">
-        <v>5.41254411223451E-6</v>
+        <v>9.03173604037676E-5</v>
       </c>
       <c r="H10" t="n">
-        <v>0.00180163808571658</v>
+        <v>1.39310535932318E-8</v>
       </c>
       <c r="I10" t="n">
         <v>50.0</v>
@@ -3388,13 +3388,13 @@
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L10" t="n">
         <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -3426,7 +3426,7 @@
         <v>4.17481529274546E-4</v>
       </c>
       <c r="I11" t="n">
-        <v>40.0</v>
+        <v>50.0</v>
       </c>
       <c r="J11" t="n">
         <v>100.0</v>
@@ -3441,33 +3441,33 @@
         <v>0.0486257928118393</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>132</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D12" t="n">
-        <v>250.0</v>
+        <v>103.0</v>
       </c>
       <c r="E12" t="n">
-        <v>26.0</v>
+        <v>19.0</v>
       </c>
       <c r="F12" t="n">
-        <v>8.8805330344482E-5</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G12" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00184132981093954</v>
+        <v>6.66551822225193E-5</v>
       </c>
       <c r="I12" t="n">
         <v>40.0</v>
@@ -3476,13 +3476,13 @@
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N12" t="n">
         <v>0.0</v>
@@ -3490,72 +3490,72 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D13" t="n">
-        <v>141.0</v>
+        <v>26.0</v>
       </c>
       <c r="E13" t="n">
-        <v>34.0</v>
+        <v>25.0</v>
       </c>
       <c r="F13" t="n">
-        <v>9.03173604037676E-5</v>
+        <v>0.234147355744326</v>
       </c>
       <c r="G13" t="n">
-        <v>5.41254411223451E-6</v>
+        <v>1.22402412262228E-4</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00187504170433014</v>
+        <v>3.8759431457377E-4</v>
       </c>
       <c r="I13" t="n">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="D14" t="n">
-        <v>103.0</v>
+        <v>250.0</v>
       </c>
       <c r="E14" t="n">
-        <v>19.0</v>
+        <v>25.0</v>
       </c>
       <c r="F14" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>9.03173604037676E-5</v>
       </c>
       <c r="G14" t="n">
-        <v>5.41254411223451E-6</v>
+        <v>3.78878087856416E-5</v>
       </c>
       <c r="H14" t="n">
-        <v>6.66551822225193E-5</v>
+        <v>0.00184132981093954</v>
       </c>
       <c r="I14" t="n">
         <v>20.0</v>
@@ -3564,39 +3564,39 @@
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.041014799154334036</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0026742305794235782</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M14" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N14" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D15" t="n">
         <v>250.0</v>
       </c>
       <c r="E15" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="F15" t="n">
-        <v>9.03173604037676E-5</v>
+        <v>8.8805330344482E-5</v>
       </c>
       <c r="G15" t="n">
-        <v>3.78878087856416E-5</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H15" t="n">
         <v>0.00184132981093954</v>
@@ -3608,13 +3608,13 @@
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -3625,25 +3625,25 @@
         <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D16" t="n">
-        <v>103.0</v>
+        <v>93.0</v>
       </c>
       <c r="E16" t="n">
-        <v>48.0</v>
+        <v>84.0</v>
       </c>
       <c r="F16" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>0.00770455162977997</v>
       </c>
       <c r="G16" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H16" t="n">
-        <v>0.00159648799018954</v>
+        <v>3.42756749960878E-4</v>
       </c>
       <c r="I16" t="n">
         <v>20.0</v>
@@ -3652,13 +3652,13 @@
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.1014799154334038</v>
+        <v>0.17885835095137423</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0</v>
+        <v>0.004011345869135358</v>
       </c>
       <c r="M16" t="n">
-        <v>0.101479915433404</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -3666,43 +3666,43 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D17" t="n">
-        <v>93.0</v>
+        <v>141.0</v>
       </c>
       <c r="E17" t="n">
-        <v>84.0</v>
+        <v>34.0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00770455162977997</v>
+        <v>9.03173604037676E-5</v>
       </c>
       <c r="G17" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H17" t="n">
-        <v>3.42756749960878E-4</v>
+        <v>0.00187504170433014</v>
       </c>
       <c r="I17" t="n">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
       <c r="J17" t="n">
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.17801268498942918</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0013371152897117859</v>
+        <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -3710,13 +3710,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D18" t="n">
         <v>103.0</v>
@@ -3754,43 +3754,43 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D19" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="E19" t="n">
         <v>48.0</v>
       </c>
-      <c r="E19" t="n">
-        <v>19.0</v>
-      </c>
       <c r="F19" t="n">
-        <v>8.9307244186841E-5</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G19" t="n">
-        <v>9.03173604037676E-5</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H19" t="n">
-        <v>0.00205785005792113</v>
+        <v>0.00159648799018954</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.041014799154334036</v>
+        <v>0.1014799154334038</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0026742305794235782</v>
+        <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>0.040169133192389</v>
+        <v>0.101479915433404</v>
       </c>
       <c r="N19" t="n">
         <v>0.0</v>
@@ -3798,28 +3798,28 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D20" t="n">
-        <v>250.0</v>
+        <v>48.0</v>
       </c>
       <c r="E20" t="n">
-        <v>27.0</v>
+        <v>19.0</v>
       </c>
       <c r="F20" t="n">
+        <v>8.9307244186841E-5</v>
+      </c>
+      <c r="G20" t="n">
         <v>9.03173604037676E-5</v>
       </c>
-      <c r="G20" t="n">
-        <v>5.41254411223451E-6</v>
-      </c>
       <c r="H20" t="n">
-        <v>0.00756459365078441</v>
+        <v>0.00205785005792113</v>
       </c>
       <c r="I20" t="n">
         <v>0.0</v>
@@ -3828,42 +3828,42 @@
         <v>0.0</v>
       </c>
       <c r="K20" t="n">
-        <v>0.05708245243128964</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L20" t="n">
         <v>0.0</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0570824524312896</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N20" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="D21" t="n">
-        <v>266.0</v>
+        <v>250.0</v>
       </c>
       <c r="E21" t="n">
-        <v>28.0</v>
+        <v>27.0</v>
       </c>
       <c r="F21" t="n">
-        <v>8.83055058344676E-5</v>
+        <v>9.03173604037676E-5</v>
       </c>
       <c r="G21" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H21" t="n">
-        <v>5.3215878608421E-5</v>
+        <v>0.00756459365078441</v>
       </c>
       <c r="I21" t="n">
         <v>0.0</v>
@@ -3872,42 +3872,42 @@
         <v>0.0</v>
       </c>
       <c r="K21" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.05708245243128964</v>
       </c>
       <c r="L21" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0570824524312896</v>
       </c>
       <c r="N21" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D22" t="n">
-        <v>250.0</v>
+        <v>266.0</v>
       </c>
       <c r="E22" t="n">
-        <v>34.0</v>
+        <v>28.0</v>
       </c>
       <c r="F22" t="n">
-        <v>9.08255730457327E-5</v>
+        <v>8.83055058344676E-5</v>
       </c>
       <c r="G22" t="n">
-        <v>1.0825088224469E-5</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0138594010247912</v>
+        <v>5.3215878608421E-5</v>
       </c>
       <c r="I22" t="n">
         <v>0.0</v>
@@ -3916,42 +3916,42 @@
         <v>0.0</v>
       </c>
       <c r="K22" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L22" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N22" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D23" t="n">
-        <v>27.0</v>
+        <v>250.0</v>
       </c>
       <c r="E23" t="n">
-        <v>15.0</v>
+        <v>34.0</v>
       </c>
       <c r="F23" t="n">
-        <v>4.90825784978946E-4</v>
+        <v>9.08255730457327E-5</v>
       </c>
       <c r="G23" t="n">
-        <v>7.52343631600598E-4</v>
+        <v>1.0825088224469E-5</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0289337904729275</v>
+        <v>0.0138594010247912</v>
       </c>
       <c r="I23" t="n">
         <v>0.0</v>
@@ -3960,13 +3960,13 @@
         <v>0.0</v>
       </c>
       <c r="K23" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L23" t="n">
         <v>0.0</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N23" t="n">
         <v>0.0</v>
@@ -3974,28 +3974,28 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D24" t="n">
-        <v>250.0</v>
+        <v>27.0</v>
       </c>
       <c r="E24" t="n">
         <v>15.0</v>
       </c>
       <c r="F24" t="n">
-        <v>8.9307244186841E-5</v>
+        <v>4.90825784978946E-4</v>
       </c>
       <c r="G24" t="n">
-        <v>9.08255730457327E-5</v>
+        <v>7.52343631600598E-4</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0118414873376809</v>
+        <v>0.0289337904729275</v>
       </c>
       <c r="I24" t="n">
         <v>0.0</v>
@@ -4018,28 +4018,28 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D25" t="n">
-        <v>93.0</v>
+        <v>250.0</v>
       </c>
       <c r="E25" t="n">
-        <v>59.0</v>
+        <v>15.0</v>
       </c>
       <c r="F25" t="n">
-        <v>9.03173604037676E-5</v>
+        <v>8.9307244186841E-5</v>
       </c>
       <c r="G25" t="n">
         <v>9.08255730457327E-5</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0171403768489598</v>
+        <v>0.0118414873376809</v>
       </c>
       <c r="I25" t="n">
         <v>0.0</v>
@@ -4048,42 +4048,42 @@
         <v>0.0</v>
       </c>
       <c r="K25" t="n">
-        <v>0.12473572938689217</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L25" t="n">
         <v>0.0</v>
       </c>
       <c r="M25" t="n">
-        <v>0.124735729386892</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N25" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
         <v>91</v>
       </c>
       <c r="D26" t="n">
-        <v>158.0</v>
+        <v>93.0</v>
       </c>
       <c r="E26" t="n">
         <v>59.0</v>
       </c>
       <c r="F26" t="n">
-        <v>8.8805330344482E-5</v>
+        <v>9.03173604037676E-5</v>
       </c>
       <c r="G26" t="n">
-        <v>5.41254411223451E-6</v>
+        <v>9.08255730457327E-5</v>
       </c>
       <c r="H26" t="n">
-        <v>0.00153668768947421</v>
+        <v>0.0171403768489598</v>
       </c>
       <c r="I26" t="n">
         <v>0.0</v>
@@ -4106,28 +4106,28 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D27" t="n">
-        <v>64.0</v>
+        <v>158.0</v>
       </c>
       <c r="E27" t="n">
-        <v>37.0</v>
+        <v>59.0</v>
       </c>
       <c r="F27" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>8.8805330344482E-5</v>
       </c>
       <c r="G27" t="n">
         <v>5.41254411223451E-6</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0144448194953813</v>
+        <v>0.00153668768947421</v>
       </c>
       <c r="I27" t="n">
         <v>0.0</v>
@@ -4136,13 +4136,13 @@
         <v>0.0</v>
       </c>
       <c r="K27" t="n">
-        <v>0.07822410147991543</v>
+        <v>0.12473572938689217</v>
       </c>
       <c r="L27" t="n">
         <v>0.0</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0782241014799154</v>
+        <v>0.124735729386892</v>
       </c>
       <c r="N27" t="n">
         <v>0.0</v>
@@ -4150,16 +4150,16 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C28" t="s">
         <v>93</v>
       </c>
       <c r="D28" t="n">
-        <v>250.0</v>
+        <v>64.0</v>
       </c>
       <c r="E28" t="n">
         <v>37.0</v>
@@ -4168,10 +4168,10 @@
         <v>8.98112524953542E-5</v>
       </c>
       <c r="G28" t="n">
-        <v>2.16501764489381E-5</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0328740366245698</v>
+        <v>0.0144448194953813</v>
       </c>
       <c r="I28" t="n">
         <v>0.0</v>
@@ -4194,28 +4194,28 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
         <v>93</v>
       </c>
-      <c r="C29" t="s">
-        <v>94</v>
-      </c>
       <c r="D29" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="E29" t="n">
         <v>37.0</v>
       </c>
-      <c r="E29" t="n">
-        <v>28.0</v>
-      </c>
       <c r="F29" t="n">
-        <v>9.28476175457405E-4</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G29" t="n">
-        <v>9.08255730457327E-5</v>
+        <v>2.16501764489381E-5</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0139149122085207</v>
+        <v>0.0328740366245698</v>
       </c>
       <c r="I29" t="n">
         <v>0.0</v>
@@ -4224,13 +4224,13 @@
         <v>0.0</v>
       </c>
       <c r="K29" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.07822410147991543</v>
       </c>
       <c r="L29" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M29" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0782241014799154</v>
       </c>
       <c r="N29" t="n">
         <v>0.0</v>
@@ -4238,28 +4238,28 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
         <v>94</v>
       </c>
       <c r="D30" t="n">
-        <v>46.0</v>
+        <v>37.0</v>
       </c>
       <c r="E30" t="n">
         <v>28.0</v>
       </c>
       <c r="F30" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>9.28476175457405E-4</v>
       </c>
       <c r="G30" t="n">
         <v>9.08255730457327E-5</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0126685742084983</v>
+        <v>0.0139149122085207</v>
       </c>
       <c r="I30" t="n">
         <v>0.0</v>
@@ -4271,39 +4271,39 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L30" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M30" t="n">
         <v>0.0591966173361522</v>
       </c>
       <c r="N30" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
         <v>94</v>
       </c>
       <c r="D31" t="n">
-        <v>35.0</v>
+        <v>46.0</v>
       </c>
       <c r="E31" t="n">
         <v>28.0</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0040277001294141</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G31" t="n">
-        <v>5.41254411223451E-6</v>
+        <v>9.08255730457327E-5</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0417860943528127</v>
+        <v>0.0126685742084983</v>
       </c>
       <c r="I31" t="n">
         <v>0.0</v>
@@ -4315,39 +4315,39 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L31" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M31" t="n">
         <v>0.0591966173361522</v>
       </c>
       <c r="N31" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>3.2710259555912E-18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D32" t="n">
-        <v>31.0</v>
+        <v>35.0</v>
       </c>
       <c r="E32" t="n">
-        <v>25.0</v>
+        <v>28.0</v>
       </c>
       <c r="F32" t="n">
-        <v>7.28059221627082E-4</v>
+        <v>0.0040277001294141</v>
       </c>
       <c r="G32" t="n">
-        <v>3.82511475459681E-4</v>
+        <v>5.41254411223451E-6</v>
       </c>
       <c r="H32" t="n">
-        <v>0.00142348782106466</v>
+        <v>0.0417860943528127</v>
       </c>
       <c r="I32" t="n">
         <v>0.0</v>
@@ -4356,13 +4356,13 @@
         <v>0.0</v>
       </c>
       <c r="K32" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M32" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N32" t="n">
         <v>0.0</v>
@@ -4370,28 +4370,28 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" t="n">
-        <v>64.0</v>
+        <v>31.0</v>
       </c>
       <c r="E33" t="n">
         <v>25.0</v>
       </c>
       <c r="F33" t="n">
-        <v>8.98112524953542E-5</v>
+        <v>7.28059221627082E-4</v>
       </c>
       <c r="G33" t="n">
-        <v>2.16501764489381E-5</v>
+        <v>3.82511475459681E-4</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0049404222516842</v>
+        <v>0.00142348782106466</v>
       </c>
       <c r="I33" t="n">
         <v>0.0</v>
@@ -4414,34 +4414,34 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" t="n">
-        <v>26.0</v>
+        <v>64.0</v>
       </c>
       <c r="E34" t="n">
         <v>25.0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.234147355744326</v>
+        <v>8.98112524953542E-5</v>
       </c>
       <c r="G34" t="n">
-        <v>1.22402412262228E-4</v>
+        <v>2.16501764489381E-5</v>
       </c>
       <c r="H34" t="n">
-        <v>3.8759431457377E-4</v>
+        <v>0.0049404222516842</v>
       </c>
       <c r="I34" t="n">
         <v>0.0</v>
       </c>
       <c r="J34" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K34" t="n">
         <v>0.052854122621564484</v>
@@ -4458,13 +4458,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
         <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D35" t="n">
         <v>120.0</v>
@@ -4535,24 +4535,24 @@
         <v>0.06765327695560254</v>
       </c>
       <c r="L36" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M36" t="n">
         <v>0.0676532769556025</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D37" t="n">
         <v>84.0</v>
@@ -4579,7 +4579,7 @@
         <v>0.09725158562367865</v>
       </c>
       <c r="L37" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M37" t="n">
         <v>0.0972515856236787</v>
@@ -4590,13 +4590,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B38" t="s">
         <v>99</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D38" t="n">
         <v>31.0</v>
@@ -4623,13 +4623,13 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M38" t="n">
         <v>0.0528541226215645</v>
       </c>
       <c r="N38" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="39">
@@ -4637,7 +4637,7 @@
         <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
         <v>98</v>
@@ -4667,7 +4667,7 @@
         <v>0.04439746300211417</v>
       </c>
       <c r="L39" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M39" t="n">
         <v>0.0443974630021142</v>
@@ -4711,13 +4711,13 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L40" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M40" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0</v>
+        <v>8.01234452659818E-18</v>
       </c>
     </row>
     <row r="41">
@@ -4755,7 +4755,7 @@
         <v>0.13530655391120508</v>
       </c>
       <c r="L41" t="n">
-        <v>0.0</v>
+        <v>9.25185853854297E-18</v>
       </c>
       <c r="M41" t="n">
         <v>0.135306553911205</v>
@@ -4769,10 +4769,10 @@
         <v>53</v>
       </c>
       <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" t="s">
         <v>84</v>
-      </c>
-      <c r="C42" t="s">
-        <v>85</v>
       </c>
       <c r="D42" t="n">
         <v>26.0</v>
@@ -4813,10 +4813,10 @@
         <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D43" t="n">
         <v>25.0</v>
@@ -4893,7 +4893,7 @@
         <v>0.0570824524312896</v>
       </c>
       <c r="N44" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="45">
@@ -4948,7 +4948,7 @@
         <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D46" t="n">
         <v>59.0</v>
@@ -4975,7 +4975,7 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L46" t="n">
-        <v>0.0</v>
+        <v>6.542051911182396E-18</v>
       </c>
       <c r="M46" t="n">
         <v>0.06553911205074</v>
@@ -4992,7 +4992,7 @@
         <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D47" t="n">
         <v>78.0</v>
@@ -5019,13 +5019,13 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L47" t="n">
-        <v>0.0</v>
+        <v>6.542051911182396E-18</v>
       </c>
       <c r="M47" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N47" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>6.5420519111824E-18</v>
       </c>
     </row>
     <row r="48">
@@ -5077,7 +5077,7 @@
         <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C49" t="s">
         <v>86</v>
@@ -5157,7 +5157,7 @@
         <v>0.0486257928118393</v>
       </c>
       <c r="N50" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="51">
@@ -5165,10 +5165,10 @@
         <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D51" t="n">
         <v>26.0</v>
@@ -5195,7 +5195,7 @@
         <v>0.05496828752642706</v>
       </c>
       <c r="L51" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M51" t="n">
         <v>0.0549682875264271</v>
@@ -5212,7 +5212,7 @@
         <v>93</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D52" t="n">
         <v>37.0</v>
@@ -5239,7 +5239,7 @@
         <v>0.05496828752642706</v>
       </c>
       <c r="L52" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M52" t="n">
         <v>0.0549682875264271</v>
@@ -5300,7 +5300,7 @@
         <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D54" t="n">
         <v>93.0</v>
@@ -5341,10 +5341,10 @@
         <v>137</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55" t="n">
         <v>250.0</v>
@@ -5385,7 +5385,7 @@
         <v>138</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C56" t="s">
         <v>106</v>
@@ -5429,7 +5429,7 @@
         <v>139</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
         <v>109</v>
@@ -5558,13 +5558,13 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B60" t="s">
         <v>78</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D60" t="e">
         <v>#NUM!</v>
@@ -5591,7 +5591,7 @@
         <v>0.0613107822410148</v>
       </c>
       <c r="L60" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M60" t="e">
         <v>#NUM!</v>
@@ -5690,13 +5690,13 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
         <v>78</v>
       </c>
       <c r="C63" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D63" t="e">
         <v>#NUM!</v>
@@ -5734,7 +5734,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B64" t="s">
         <v>78</v>
@@ -5778,7 +5778,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
         <v>78</v>
@@ -5828,7 +5828,7 @@
         <v>78</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D66" t="e">
         <v>#NUM!</v>
@@ -5872,7 +5872,7 @@
         <v>78</v>
       </c>
       <c r="C67" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D67" t="e">
         <v>#NUM!</v>
@@ -6072,10 +6072,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K71" t="n">
-        <v>0.4945031712473573</v>
+        <v>0.48477801268498943</v>
       </c>
       <c r="L71" t="n">
-        <v>0.015709128886722563</v>
+        <v>0.0020056729345676876</v>
       </c>
       <c r="M71" t="e">
         <v>#NUM!</v>

</xml_diff>